<commit_message>
Versión 0 de ComparacionTextosSpacyNLP
</commit_message>
<xml_diff>
--- a/documentos/datasetNLP.xlsx
+++ b/documentos/datasetNLP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programas propios\Python\CompararTextos\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68AC6DD9-9092-4BE1-93A8-71C04C636F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A301BA5-085D-43E4-8952-FD48CCEC54DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>Simil. Calculada (%)</t>
   </si>
   <si>
-    <t>Convalidable</t>
-  </si>
-  <si>
     <t>Eficiencia (%)</t>
   </si>
   <si>
@@ -1347,17 +1344,33 @@
   </si>
   <si>
     <t>1 a 5</t>
+  </si>
+  <si>
+    <t>Convalidable calculado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1380,9 +1393,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1690,41 +1705,48 @@
   <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K101" sqref="K2:K101"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="17.08984375" customWidth="1"/>
+    <col min="7" max="7" width="18.26953125" customWidth="1"/>
+    <col min="8" max="8" width="22.08984375" customWidth="1"/>
+    <col min="9" max="9" width="16.36328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>437</v>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -1732,25 +1754,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
       </c>
       <c r="F2">
         <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="I2">
         <v>97.082186966186001</v>
@@ -1765,25 +1787,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
       </c>
       <c r="F3">
         <v>60</v>
       </c>
       <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
         <v>19</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
       </c>
       <c r="I3">
         <v>70.357357157851993</v>
@@ -1798,25 +1820,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
       </c>
       <c r="F4">
         <v>75</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I4">
         <v>90.038540182426004</v>
@@ -1831,25 +1853,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
       </c>
       <c r="F5">
         <v>78</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I5">
         <v>83.104919136350006</v>
@@ -1864,25 +1886,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
         <v>31</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>32</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>33</v>
-      </c>
-      <c r="E6" t="s">
-        <v>34</v>
       </c>
       <c r="F6">
         <v>55</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I6">
         <v>71.080006709215994</v>
@@ -1897,25 +1919,25 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
         <v>36</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>37</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>38</v>
-      </c>
-      <c r="E7" t="s">
-        <v>39</v>
       </c>
       <c r="F7">
         <v>85</v>
       </c>
       <c r="G7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I7">
         <v>89.111316169006002</v>
@@ -1930,25 +1952,25 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
         <v>41</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>42</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>43</v>
-      </c>
-      <c r="E8" t="s">
-        <v>44</v>
       </c>
       <c r="F8">
         <v>77</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I8">
         <v>96.957501935604995</v>
@@ -1963,25 +1985,25 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
         <v>46</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>47</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>48</v>
-      </c>
-      <c r="E9" t="s">
-        <v>49</v>
       </c>
       <c r="F9">
         <v>79</v>
       </c>
       <c r="G9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I9">
         <v>88.596679645601995</v>
@@ -1996,25 +2018,25 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
         <v>51</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>52</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>53</v>
-      </c>
-      <c r="E10" t="s">
-        <v>54</v>
       </c>
       <c r="F10">
         <v>80</v>
       </c>
       <c r="G10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I10">
         <v>93.244782276148996</v>
@@ -2029,25 +2051,25 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
         <v>56</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>57</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>58</v>
-      </c>
-      <c r="E11" t="s">
-        <v>59</v>
       </c>
       <c r="F11">
         <v>83</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I11">
         <v>98.077029362665996</v>
@@ -2062,25 +2084,25 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" t="s">
         <v>60</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>61</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>62</v>
-      </c>
-      <c r="E12" t="s">
-        <v>63</v>
       </c>
       <c r="F12">
         <v>82</v>
       </c>
       <c r="G12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I12">
         <v>97.694706866130005</v>
@@ -2095,25 +2117,25 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" t="s">
         <v>65</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>66</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>67</v>
-      </c>
-      <c r="E13" t="s">
-        <v>68</v>
       </c>
       <c r="F13">
         <v>79</v>
       </c>
       <c r="G13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I13">
         <v>99.487144836371996</v>
@@ -2128,25 +2150,25 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
         <v>70</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>71</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>72</v>
-      </c>
-      <c r="E14" t="s">
-        <v>73</v>
       </c>
       <c r="F14">
         <v>75</v>
       </c>
       <c r="G14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I14">
         <v>88.147989594231007</v>
@@ -2161,25 +2183,25 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" t="s">
         <v>75</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>76</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>77</v>
-      </c>
-      <c r="E15" t="s">
-        <v>78</v>
       </c>
       <c r="F15">
         <v>81</v>
       </c>
       <c r="G15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I15">
         <v>80.847884493706005</v>
@@ -2194,25 +2216,25 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" t="s">
         <v>80</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>81</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>82</v>
-      </c>
-      <c r="E16" t="s">
-        <v>83</v>
       </c>
       <c r="F16">
         <v>84</v>
       </c>
       <c r="G16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I16">
         <v>86.250709938892996</v>
@@ -2227,25 +2249,25 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" t="s">
         <v>85</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>86</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>87</v>
-      </c>
-      <c r="E17" t="s">
-        <v>88</v>
       </c>
       <c r="F17">
         <v>77</v>
       </c>
       <c r="G17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I17">
         <v>88.351152674757003</v>
@@ -2260,25 +2282,25 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" t="s">
         <v>90</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>91</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>92</v>
-      </c>
-      <c r="E18" t="s">
-        <v>93</v>
       </c>
       <c r="F18">
         <v>76</v>
       </c>
       <c r="G18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I18">
         <v>98.257113115525996</v>
@@ -2293,25 +2315,25 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" t="s">
         <v>95</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>96</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>97</v>
-      </c>
-      <c r="E19" t="s">
-        <v>98</v>
       </c>
       <c r="F19">
         <v>83</v>
       </c>
       <c r="G19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I19">
         <v>98.398500895759994</v>
@@ -2326,25 +2348,25 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" t="s">
         <v>100</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>101</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>102</v>
-      </c>
-      <c r="E20" t="s">
-        <v>103</v>
       </c>
       <c r="F20">
         <v>80</v>
       </c>
       <c r="G20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I20">
         <v>78.793688857454995</v>
@@ -2359,25 +2381,25 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" t="s">
         <v>105</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>106</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>107</v>
-      </c>
-      <c r="E21" t="s">
-        <v>108</v>
       </c>
       <c r="F21">
         <v>78</v>
       </c>
       <c r="G21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I21">
         <v>95.544897691661006</v>
@@ -2392,25 +2414,25 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" t="s">
         <v>110</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>111</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>112</v>
-      </c>
-      <c r="E22" t="s">
-        <v>113</v>
       </c>
       <c r="F22">
         <v>85</v>
       </c>
       <c r="G22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I22">
         <v>77.128372040450003</v>
@@ -2425,25 +2447,25 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" t="s">
         <v>115</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>116</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>117</v>
-      </c>
-      <c r="E23" t="s">
-        <v>118</v>
       </c>
       <c r="F23">
         <v>81</v>
       </c>
       <c r="G23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I23">
         <v>92.180970566171993</v>
@@ -2458,25 +2480,25 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" t="s">
         <v>120</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>121</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>122</v>
-      </c>
-      <c r="E24" t="s">
-        <v>123</v>
       </c>
       <c r="F24">
         <v>86</v>
       </c>
       <c r="G24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I24">
         <v>97.336672824855995</v>
@@ -2491,25 +2513,25 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" t="s">
         <v>87</v>
       </c>
-      <c r="C25" t="s">
-        <v>88</v>
-      </c>
       <c r="D25" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" t="s">
         <v>85</v>
-      </c>
-      <c r="E25" t="s">
-        <v>86</v>
       </c>
       <c r="F25">
         <v>79</v>
       </c>
       <c r="G25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I25">
         <v>86.351152674757003</v>
@@ -2524,25 +2546,25 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" t="s">
         <v>125</v>
       </c>
-      <c r="C26" t="s">
-        <v>126</v>
-      </c>
       <c r="D26" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" t="s">
         <v>65</v>
-      </c>
-      <c r="E26" t="s">
-        <v>66</v>
       </c>
       <c r="F26">
         <v>87</v>
       </c>
       <c r="G26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I26">
         <v>89.487144836371996</v>
@@ -2557,25 +2579,25 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" t="s">
         <v>128</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>129</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>130</v>
-      </c>
-      <c r="E27" t="s">
-        <v>131</v>
       </c>
       <c r="F27">
         <v>82</v>
       </c>
       <c r="G27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I27">
         <v>99.493485473061</v>
@@ -2590,25 +2612,25 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C28" t="s">
         <v>133</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>134</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>135</v>
-      </c>
-      <c r="E28" t="s">
-        <v>136</v>
       </c>
       <c r="F28">
         <v>80</v>
       </c>
       <c r="G28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I28">
         <v>78.448548752769</v>
@@ -2623,25 +2645,25 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>137</v>
+      </c>
+      <c r="C29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" t="s">
         <v>138</v>
-      </c>
-      <c r="C29" t="s">
-        <v>73</v>
-      </c>
-      <c r="D29" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" t="s">
-        <v>139</v>
       </c>
       <c r="F29">
         <v>75</v>
       </c>
       <c r="G29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I29">
         <v>83.147989594231007</v>
@@ -2656,25 +2678,25 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>140</v>
+      </c>
+      <c r="C30" t="s">
         <v>141</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>142</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>143</v>
-      </c>
-      <c r="E30" t="s">
-        <v>144</v>
       </c>
       <c r="F30">
         <v>88</v>
       </c>
       <c r="G30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I30">
         <v>97.416218901413004</v>
@@ -2689,25 +2711,25 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>145</v>
+      </c>
+      <c r="C31" t="s">
         <v>146</v>
       </c>
-      <c r="C31" t="s">
-        <v>147</v>
-      </c>
       <c r="D31" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" t="s">
         <v>51</v>
-      </c>
-      <c r="E31" t="s">
-        <v>52</v>
       </c>
       <c r="F31">
         <v>83</v>
       </c>
       <c r="G31" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I31">
         <v>97.876185562724999</v>
@@ -2722,25 +2744,25 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>148</v>
+      </c>
+      <c r="C32" t="s">
         <v>149</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>150</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>151</v>
-      </c>
-      <c r="E32" t="s">
-        <v>152</v>
       </c>
       <c r="F32">
         <v>79</v>
       </c>
       <c r="G32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I32">
         <v>95.980000439788</v>
@@ -2755,25 +2777,25 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>153</v>
+      </c>
+      <c r="C33" t="s">
         <v>154</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>155</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>156</v>
-      </c>
-      <c r="E33" t="s">
-        <v>157</v>
       </c>
       <c r="F33">
         <v>82</v>
       </c>
       <c r="G33" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I33">
         <v>90.617652881200002</v>
@@ -2788,25 +2810,25 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
+        <v>158</v>
+      </c>
+      <c r="C34" t="s">
         <v>159</v>
       </c>
-      <c r="C34" t="s">
-        <v>160</v>
-      </c>
       <c r="D34" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" t="s">
         <v>65</v>
-      </c>
-      <c r="E34" t="s">
-        <v>66</v>
       </c>
       <c r="F34">
         <v>85</v>
       </c>
       <c r="G34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I34">
         <v>91.652535998957006</v>
@@ -2821,25 +2843,25 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
+        <v>161</v>
+      </c>
+      <c r="C35" t="s">
         <v>162</v>
       </c>
-      <c r="C35" t="s">
-        <v>163</v>
-      </c>
       <c r="D35" t="s">
+        <v>121</v>
+      </c>
+      <c r="E35" t="s">
         <v>122</v>
-      </c>
-      <c r="E35" t="s">
-        <v>123</v>
       </c>
       <c r="F35">
         <v>83</v>
       </c>
       <c r="G35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I35">
         <v>79.748716993266996</v>
@@ -2854,25 +2876,25 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>164</v>
+      </c>
+      <c r="C36" t="s">
         <v>165</v>
       </c>
-      <c r="C36" t="s">
-        <v>166</v>
-      </c>
       <c r="D36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E36" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F36">
         <v>79</v>
       </c>
       <c r="G36" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I36">
         <v>91.161441048011</v>
@@ -2887,25 +2909,25 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>167</v>
+      </c>
+      <c r="C37" t="s">
         <v>168</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>169</v>
       </c>
-      <c r="D37" t="s">
-        <v>170</v>
-      </c>
       <c r="E37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F37">
         <v>81</v>
       </c>
       <c r="G37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I37">
         <v>71.253909822861999</v>
@@ -2920,25 +2942,25 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D38" t="s">
+        <v>161</v>
+      </c>
+      <c r="E38" t="s">
         <v>162</v>
-      </c>
-      <c r="E38" t="s">
-        <v>163</v>
       </c>
       <c r="F38">
         <v>83</v>
       </c>
       <c r="G38" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I38">
         <v>99.748716993266996</v>
@@ -2953,25 +2975,25 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
+        <v>173</v>
+      </c>
+      <c r="C39" t="s">
         <v>174</v>
       </c>
-      <c r="C39" t="s">
-        <v>175</v>
-      </c>
       <c r="D39" t="s">
+        <v>47</v>
+      </c>
+      <c r="E39" t="s">
         <v>48</v>
-      </c>
-      <c r="E39" t="s">
-        <v>49</v>
       </c>
       <c r="F39">
         <v>84</v>
       </c>
       <c r="G39" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I39">
         <v>96.554801926655998</v>
@@ -2986,25 +3008,25 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
+        <v>176</v>
+      </c>
+      <c r="C40" t="s">
         <v>177</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>178</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>179</v>
-      </c>
-      <c r="E40" t="s">
-        <v>180</v>
       </c>
       <c r="F40">
         <v>82</v>
       </c>
       <c r="G40" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I40">
         <v>72.797733716878</v>
@@ -3019,25 +3041,25 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
+        <v>181</v>
+      </c>
+      <c r="C41" t="s">
         <v>182</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>183</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>184</v>
-      </c>
-      <c r="E41" t="s">
-        <v>185</v>
       </c>
       <c r="F41">
         <v>80</v>
       </c>
       <c r="G41" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H41" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I41">
         <v>92.679406690909005</v>
@@ -3052,25 +3074,25 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
+        <v>186</v>
+      </c>
+      <c r="C42" t="s">
         <v>187</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>188</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>189</v>
-      </c>
-      <c r="E42" t="s">
-        <v>190</v>
       </c>
       <c r="F42">
         <v>86</v>
       </c>
       <c r="G42" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I42">
         <v>85.052098947920001</v>
@@ -3085,25 +3107,25 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>191</v>
+      </c>
+      <c r="C43" t="s">
         <v>192</v>
       </c>
-      <c r="C43" t="s">
-        <v>193</v>
-      </c>
       <c r="D43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E43" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F43">
         <v>81</v>
       </c>
       <c r="G43" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I43">
         <v>97.845172564573005</v>
@@ -3118,25 +3140,25 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>194</v>
+      </c>
+      <c r="C44" t="s">
         <v>195</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>196</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>197</v>
-      </c>
-      <c r="E44" t="s">
-        <v>198</v>
       </c>
       <c r="F44">
         <v>84</v>
       </c>
       <c r="G44" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I44">
         <v>85.433706733337999</v>
@@ -3151,25 +3173,25 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>199</v>
+      </c>
+      <c r="C45" t="s">
         <v>200</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>201</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>202</v>
-      </c>
-      <c r="E45" t="s">
-        <v>203</v>
       </c>
       <c r="F45">
         <v>82</v>
       </c>
       <c r="G45" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I45">
         <v>77.338491412920007</v>
@@ -3184,25 +3206,25 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F46">
         <v>85</v>
       </c>
       <c r="G46" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H46" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I46">
         <v>85.802377676188996</v>
@@ -3217,25 +3239,25 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
+        <v>206</v>
+      </c>
+      <c r="C47" t="s">
         <v>207</v>
       </c>
-      <c r="C47" t="s">
-        <v>208</v>
-      </c>
       <c r="D47" t="s">
+        <v>145</v>
+      </c>
+      <c r="E47" t="s">
         <v>146</v>
-      </c>
-      <c r="E47" t="s">
-        <v>147</v>
       </c>
       <c r="F47">
         <v>87</v>
       </c>
       <c r="G47" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H47" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I47">
         <v>94.506130496926005</v>
@@ -3250,25 +3272,25 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
+        <v>209</v>
+      </c>
+      <c r="C48" t="s">
         <v>210</v>
       </c>
-      <c r="C48" t="s">
-        <v>211</v>
-      </c>
       <c r="D48" t="s">
+        <v>114</v>
+      </c>
+      <c r="E48" t="s">
         <v>115</v>
-      </c>
-      <c r="E48" t="s">
-        <v>116</v>
       </c>
       <c r="F48">
         <v>81</v>
       </c>
       <c r="G48" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I48">
         <v>91.560874989474996</v>
@@ -3283,25 +3305,25 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
+        <v>212</v>
+      </c>
+      <c r="C49" t="s">
         <v>213</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>214</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>215</v>
-      </c>
-      <c r="E49" t="s">
-        <v>216</v>
       </c>
       <c r="F49">
         <v>83</v>
       </c>
       <c r="G49" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H49" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I49">
         <v>92.815142918283996</v>
@@ -3316,25 +3338,25 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
+        <v>111</v>
+      </c>
+      <c r="C50" t="s">
         <v>112</v>
       </c>
-      <c r="C50" t="s">
-        <v>113</v>
-      </c>
       <c r="D50" t="s">
+        <v>217</v>
+      </c>
+      <c r="E50" t="s">
         <v>218</v>
-      </c>
-      <c r="E50" t="s">
-        <v>219</v>
       </c>
       <c r="F50">
         <v>85</v>
       </c>
       <c r="G50" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H50" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I50">
         <v>96.814844880365001</v>
@@ -3349,25 +3371,25 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
+        <v>220</v>
+      </c>
+      <c r="C51" t="s">
         <v>221</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>222</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>223</v>
-      </c>
-      <c r="E51" t="s">
-        <v>224</v>
       </c>
       <c r="F51">
         <v>82</v>
       </c>
       <c r="G51" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I51">
         <v>82.776766135559996</v>
@@ -3382,25 +3404,25 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
+        <v>225</v>
+      </c>
+      <c r="C52" t="s">
         <v>226</v>
       </c>
-      <c r="C52" t="s">
-        <v>227</v>
-      </c>
       <c r="D52" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E52" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F52">
         <v>83</v>
       </c>
       <c r="G52" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I52">
         <v>88.942203175567002</v>
@@ -3415,25 +3437,25 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
+        <v>228</v>
+      </c>
+      <c r="C53" t="s">
         <v>229</v>
       </c>
-      <c r="C53" t="s">
-        <v>230</v>
-      </c>
       <c r="D53" t="s">
+        <v>199</v>
+      </c>
+      <c r="E53" t="s">
         <v>200</v>
-      </c>
-      <c r="E53" t="s">
-        <v>201</v>
       </c>
       <c r="F53">
         <v>84</v>
       </c>
       <c r="G53" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H53" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I53">
         <v>88.235931704194996</v>
@@ -3448,25 +3470,25 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
+        <v>231</v>
+      </c>
+      <c r="C54" t="s">
         <v>232</v>
       </c>
-      <c r="C54" t="s">
-        <v>233</v>
-      </c>
       <c r="D54" t="s">
+        <v>150</v>
+      </c>
+      <c r="E54" t="s">
         <v>151</v>
-      </c>
-      <c r="E54" t="s">
-        <v>152</v>
       </c>
       <c r="F54">
         <v>80</v>
       </c>
       <c r="G54" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H54" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I54">
         <v>93.210673642987999</v>
@@ -3481,25 +3503,25 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
+        <v>234</v>
+      </c>
+      <c r="C55" t="s">
         <v>235</v>
       </c>
-      <c r="C55" t="s">
-        <v>236</v>
-      </c>
       <c r="D55" t="s">
+        <v>181</v>
+      </c>
+      <c r="E55" t="s">
         <v>182</v>
-      </c>
-      <c r="E55" t="s">
-        <v>183</v>
       </c>
       <c r="F55">
         <v>86</v>
       </c>
       <c r="G55" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I55">
         <v>99.967784075584007</v>
@@ -3514,25 +3536,25 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
+        <v>237</v>
+      </c>
+      <c r="C56" t="s">
         <v>238</v>
       </c>
-      <c r="C56" t="s">
-        <v>239</v>
-      </c>
       <c r="D56" t="s">
+        <v>231</v>
+      </c>
+      <c r="E56" t="s">
         <v>232</v>
-      </c>
-      <c r="E56" t="s">
-        <v>233</v>
       </c>
       <c r="F56">
         <v>82</v>
       </c>
       <c r="G56" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H56" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I56">
         <v>83.765077660109</v>
@@ -3547,25 +3569,25 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
+        <v>240</v>
+      </c>
+      <c r="C57" t="s">
         <v>241</v>
       </c>
-      <c r="C57" t="s">
-        <v>242</v>
-      </c>
       <c r="D57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E57" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F57">
         <v>50</v>
       </c>
       <c r="G57" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I57">
         <v>65.887383014801003</v>
@@ -3580,25 +3602,25 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
+        <v>243</v>
+      </c>
+      <c r="C58" t="s">
         <v>244</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>245</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>246</v>
-      </c>
-      <c r="E58" t="s">
-        <v>247</v>
       </c>
       <c r="F58">
         <v>72</v>
       </c>
       <c r="G58" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H58" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I58">
         <v>95.442488520837998</v>
@@ -3613,25 +3635,25 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
+        <v>248</v>
+      </c>
+      <c r="C59" t="s">
         <v>249</v>
       </c>
-      <c r="C59" t="s">
-        <v>250</v>
-      </c>
       <c r="D59" t="s">
+        <v>50</v>
+      </c>
+      <c r="E59" t="s">
         <v>51</v>
-      </c>
-      <c r="E59" t="s">
-        <v>52</v>
       </c>
       <c r="F59">
         <v>68</v>
       </c>
       <c r="G59" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H59" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I59">
         <v>86.767728055879999</v>
@@ -3646,25 +3668,25 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
+        <v>251</v>
+      </c>
+      <c r="C60" t="s">
         <v>252</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>253</v>
       </c>
-      <c r="D60" t="s">
-        <v>254</v>
-      </c>
       <c r="E60" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F60">
         <v>74</v>
       </c>
       <c r="G60" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H60" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I60">
         <v>62.350008257851002</v>
@@ -3679,25 +3701,25 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C61" t="s">
+        <v>255</v>
+      </c>
+      <c r="D61" t="s">
         <v>256</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>257</v>
-      </c>
-      <c r="E61" t="s">
-        <v>258</v>
       </c>
       <c r="F61">
         <v>70</v>
       </c>
       <c r="G61" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H61" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I61">
         <v>80.764074333313005</v>
@@ -3712,25 +3734,25 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C62" t="s">
+        <v>259</v>
+      </c>
+      <c r="D62" t="s">
         <v>260</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>261</v>
-      </c>
-      <c r="E62" t="s">
-        <v>262</v>
       </c>
       <c r="F62">
         <v>68</v>
       </c>
       <c r="G62" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H62" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I62">
         <v>94.516543643831994</v>
@@ -3745,25 +3767,25 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C63" t="s">
+        <v>263</v>
+      </c>
+      <c r="D63" t="s">
+        <v>134</v>
+      </c>
+      <c r="E63" t="s">
         <v>264</v>
-      </c>
-      <c r="D63" t="s">
-        <v>135</v>
-      </c>
-      <c r="E63" t="s">
-        <v>265</v>
       </c>
       <c r="F63">
         <v>71</v>
       </c>
       <c r="G63" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H63" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I63">
         <v>87.530256696164003</v>
@@ -3778,25 +3800,25 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
+        <v>266</v>
+      </c>
+      <c r="C64" t="s">
         <v>267</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>268</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>269</v>
-      </c>
-      <c r="E64" t="s">
-        <v>270</v>
       </c>
       <c r="F64">
         <v>73</v>
       </c>
       <c r="G64" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H64" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I64">
         <v>86.433963212313998</v>
@@ -3811,25 +3833,25 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
+        <v>271</v>
+      </c>
+      <c r="C65" t="s">
         <v>272</v>
       </c>
-      <c r="C65" t="s">
-        <v>273</v>
-      </c>
       <c r="D65" t="s">
+        <v>201</v>
+      </c>
+      <c r="E65" t="s">
         <v>202</v>
-      </c>
-      <c r="E65" t="s">
-        <v>203</v>
       </c>
       <c r="F65">
         <v>76</v>
       </c>
       <c r="G65" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H65" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I65">
         <v>96.319187088906006</v>
@@ -3844,25 +3866,25 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
+        <v>274</v>
+      </c>
+      <c r="C66" t="s">
         <v>275</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
+        <v>99</v>
+      </c>
+      <c r="E66" t="s">
         <v>276</v>
-      </c>
-      <c r="D66" t="s">
-        <v>100</v>
-      </c>
-      <c r="E66" t="s">
-        <v>277</v>
       </c>
       <c r="F66">
         <v>70</v>
       </c>
       <c r="G66" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H66" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I66">
         <v>84.263155279963001</v>
@@ -3877,25 +3899,25 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C67" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D67" t="s">
+        <v>111</v>
+      </c>
+      <c r="E67" t="s">
         <v>112</v>
-      </c>
-      <c r="E67" t="s">
-        <v>113</v>
       </c>
       <c r="F67">
         <v>68</v>
       </c>
       <c r="G67" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H67" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I67">
         <v>88.725666810651006</v>
@@ -3910,25 +3932,25 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
+        <v>280</v>
+      </c>
+      <c r="C68" t="s">
         <v>281</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>282</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>283</v>
-      </c>
-      <c r="E68" t="s">
-        <v>284</v>
       </c>
       <c r="F68">
         <v>65</v>
       </c>
       <c r="G68" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H68" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I68">
         <v>73.586692571547999</v>
@@ -3943,25 +3965,25 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
+        <v>285</v>
+      </c>
+      <c r="C69" t="s">
         <v>286</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>287</v>
       </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
         <v>288</v>
-      </c>
-      <c r="E69" t="s">
-        <v>289</v>
       </c>
       <c r="F69">
         <v>70</v>
       </c>
       <c r="G69" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H69" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I69">
         <v>91.495916922166998</v>
@@ -3976,25 +3998,25 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
+        <v>290</v>
+      </c>
+      <c r="C70" t="s">
         <v>291</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>292</v>
       </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
         <v>293</v>
-      </c>
-      <c r="E70" t="s">
-        <v>294</v>
       </c>
       <c r="F70">
         <v>68</v>
       </c>
       <c r="G70" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H70" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I70">
         <v>73.978232681669994</v>
@@ -4009,25 +4031,25 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
+        <v>295</v>
+      </c>
+      <c r="C71" t="s">
         <v>296</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
         <v>297</v>
       </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
         <v>298</v>
-      </c>
-      <c r="E71" t="s">
-        <v>299</v>
       </c>
       <c r="F71">
         <v>72</v>
       </c>
       <c r="G71" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H71" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I71">
         <v>74.577845053629005</v>
@@ -4042,25 +4064,25 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C72" t="s">
+        <v>300</v>
+      </c>
+      <c r="D72" t="s">
+        <v>71</v>
+      </c>
+      <c r="E72" t="s">
         <v>301</v>
-      </c>
-      <c r="D72" t="s">
-        <v>72</v>
-      </c>
-      <c r="E72" t="s">
-        <v>302</v>
       </c>
       <c r="F72">
         <v>74</v>
       </c>
       <c r="G72" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H72" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I72">
         <v>82.174729113999007</v>
@@ -4075,25 +4097,25 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
+        <v>303</v>
+      </c>
+      <c r="C73" t="s">
         <v>304</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
         <v>305</v>
       </c>
-      <c r="D73" t="s">
+      <c r="E73" t="s">
         <v>306</v>
-      </c>
-      <c r="E73" t="s">
-        <v>307</v>
       </c>
       <c r="F73">
         <v>68</v>
       </c>
       <c r="G73" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H73" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I73">
         <v>72.259466796593003</v>
@@ -4108,25 +4130,25 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C74" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D74" t="s">
+        <v>285</v>
+      </c>
+      <c r="E74" t="s">
         <v>286</v>
-      </c>
-      <c r="E74" t="s">
-        <v>287</v>
       </c>
       <c r="F74">
         <v>71</v>
       </c>
       <c r="G74" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H74" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I74">
         <v>81.955131201504003</v>
@@ -4141,25 +4163,25 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
+        <v>310</v>
+      </c>
+      <c r="C75" t="s">
         <v>311</v>
       </c>
-      <c r="C75" t="s">
+      <c r="D75" t="s">
         <v>312</v>
       </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
         <v>313</v>
-      </c>
-      <c r="E75" t="s">
-        <v>314</v>
       </c>
       <c r="F75">
         <v>69</v>
       </c>
       <c r="G75" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H75" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I75">
         <v>76.176146495967004</v>
@@ -4174,25 +4196,25 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
+        <v>315</v>
+      </c>
+      <c r="C76" t="s">
         <v>316</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D76" t="s">
         <v>317</v>
       </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
         <v>318</v>
-      </c>
-      <c r="E76" t="s">
-        <v>319</v>
       </c>
       <c r="F76">
         <v>73</v>
       </c>
       <c r="G76" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H76" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I76">
         <v>84.238345745244999</v>
@@ -4207,25 +4229,25 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
+        <v>320</v>
+      </c>
+      <c r="C77" t="s">
         <v>321</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
         <v>322</v>
       </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
         <v>323</v>
-      </c>
-      <c r="E77" t="s">
-        <v>324</v>
       </c>
       <c r="F77">
         <v>67</v>
       </c>
       <c r="G77" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H77" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I77">
         <v>74.564644786707007</v>
@@ -4240,25 +4262,25 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
+        <v>325</v>
+      </c>
+      <c r="C78" t="s">
         <v>326</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
+        <v>142</v>
+      </c>
+      <c r="E78" t="s">
         <v>327</v>
-      </c>
-      <c r="D78" t="s">
-        <v>143</v>
-      </c>
-      <c r="E78" t="s">
-        <v>328</v>
       </c>
       <c r="F78">
         <v>85</v>
       </c>
       <c r="G78" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H78" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I78">
         <v>96.255830826847003</v>
@@ -4273,25 +4295,25 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
+        <v>329</v>
+      </c>
+      <c r="C79" t="s">
         <v>330</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
+        <v>66</v>
+      </c>
+      <c r="E79" t="s">
         <v>331</v>
-      </c>
-      <c r="D79" t="s">
-        <v>67</v>
-      </c>
-      <c r="E79" t="s">
-        <v>332</v>
       </c>
       <c r="F79">
         <v>78</v>
       </c>
       <c r="G79" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H79" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I79">
         <v>96.339122433086999</v>
@@ -4306,25 +4328,25 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C80" t="s">
+        <v>333</v>
+      </c>
+      <c r="D80" t="s">
         <v>334</v>
       </c>
-      <c r="D80" t="s">
+      <c r="E80" t="s">
         <v>335</v>
-      </c>
-      <c r="E80" t="s">
-        <v>336</v>
       </c>
       <c r="F80">
         <v>82</v>
       </c>
       <c r="G80" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H80" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I80">
         <v>95.925795196403001</v>
@@ -4339,25 +4361,25 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C81" t="s">
+        <v>337</v>
+      </c>
+      <c r="D81" t="s">
+        <v>57</v>
+      </c>
+      <c r="E81" t="s">
         <v>338</v>
-      </c>
-      <c r="D81" t="s">
-        <v>58</v>
-      </c>
-      <c r="E81" t="s">
-        <v>339</v>
       </c>
       <c r="F81">
         <v>79</v>
       </c>
       <c r="G81" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H81" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I81">
         <v>89.801957002809999</v>
@@ -4372,25 +4394,25 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
+        <v>340</v>
+      </c>
+      <c r="C82" t="s">
         <v>341</v>
       </c>
-      <c r="C82" t="s">
+      <c r="D82" t="s">
         <v>342</v>
       </c>
-      <c r="D82" t="s">
+      <c r="E82" t="s">
         <v>343</v>
-      </c>
-      <c r="E82" t="s">
-        <v>344</v>
       </c>
       <c r="F82">
         <v>75</v>
       </c>
       <c r="G82" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H82" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I82">
         <v>94.043368861803003</v>
@@ -4405,25 +4427,25 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
+        <v>345</v>
+      </c>
+      <c r="C83" t="s">
         <v>346</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
         <v>347</v>
       </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>348</v>
-      </c>
-      <c r="E83" t="s">
-        <v>349</v>
       </c>
       <c r="F83">
         <v>88</v>
       </c>
       <c r="G83" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H83" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I83">
         <v>99.711269030934005</v>
@@ -4438,25 +4460,25 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C84" t="s">
+        <v>350</v>
+      </c>
+      <c r="D84" t="s">
+        <v>155</v>
+      </c>
+      <c r="E84" t="s">
         <v>351</v>
-      </c>
-      <c r="D84" t="s">
-        <v>156</v>
-      </c>
-      <c r="E84" t="s">
-        <v>352</v>
       </c>
       <c r="F84">
         <v>80</v>
       </c>
       <c r="G84" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H84" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I84">
         <v>99.575278102934007</v>
@@ -4471,25 +4493,25 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
+        <v>353</v>
+      </c>
+      <c r="C85" t="s">
         <v>354</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D85" t="s">
         <v>355</v>
       </c>
-      <c r="D85" t="s">
+      <c r="E85" t="s">
         <v>356</v>
-      </c>
-      <c r="E85" t="s">
-        <v>357</v>
       </c>
       <c r="F85">
         <v>84</v>
       </c>
       <c r="G85" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H85" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I85">
         <v>91.058375519056</v>
@@ -4504,25 +4526,25 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
+        <v>358</v>
+      </c>
+      <c r="C86" t="s">
         <v>359</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
         <v>360</v>
       </c>
-      <c r="D86" t="s">
+      <c r="E86" t="s">
         <v>361</v>
-      </c>
-      <c r="E86" t="s">
-        <v>362</v>
       </c>
       <c r="F86">
         <v>76</v>
       </c>
       <c r="G86" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H86" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I86">
         <v>92.062136562312006</v>
@@ -4537,25 +4559,25 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
+        <v>363</v>
+      </c>
+      <c r="C87" t="s">
         <v>364</v>
       </c>
-      <c r="C87" t="s">
+      <c r="D87" t="s">
         <v>365</v>
       </c>
-      <c r="D87" t="s">
+      <c r="E87" t="s">
         <v>366</v>
-      </c>
-      <c r="E87" t="s">
-        <v>367</v>
       </c>
       <c r="F87">
         <v>81</v>
       </c>
       <c r="G87" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="H87" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I87">
         <v>92.909263587957</v>
@@ -4570,25 +4592,25 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
+        <v>368</v>
+      </c>
+      <c r="C88" t="s">
         <v>369</v>
       </c>
-      <c r="C88" t="s">
+      <c r="D88" t="s">
         <v>370</v>
       </c>
-      <c r="D88" t="s">
+      <c r="E88" t="s">
         <v>371</v>
-      </c>
-      <c r="E88" t="s">
-        <v>372</v>
       </c>
       <c r="F88">
         <v>79</v>
       </c>
       <c r="G88" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H88" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I88">
         <v>92.285541311714994</v>
@@ -4603,25 +4625,25 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
+        <v>373</v>
+      </c>
+      <c r="C89" t="s">
         <v>374</v>
       </c>
-      <c r="C89" t="s">
+      <c r="D89" t="s">
         <v>375</v>
       </c>
-      <c r="D89" t="s">
+      <c r="E89" t="s">
         <v>376</v>
-      </c>
-      <c r="E89" t="s">
-        <v>377</v>
       </c>
       <c r="F89">
         <v>77</v>
       </c>
       <c r="G89" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H89" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I89">
         <v>83.563133488348996</v>
@@ -4636,25 +4658,25 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
+        <v>378</v>
+      </c>
+      <c r="C90" t="s">
         <v>379</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D90" t="s">
+        <v>280</v>
+      </c>
+      <c r="E90" t="s">
         <v>380</v>
-      </c>
-      <c r="D90" t="s">
-        <v>281</v>
-      </c>
-      <c r="E90" t="s">
-        <v>381</v>
       </c>
       <c r="F90">
         <v>86</v>
       </c>
       <c r="G90" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H90" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I90">
         <v>81.378985754973002</v>
@@ -4669,25 +4691,25 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
+        <v>382</v>
+      </c>
+      <c r="C91" t="s">
         <v>383</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
+        <v>71</v>
+      </c>
+      <c r="E91" t="s">
         <v>384</v>
-      </c>
-      <c r="D91" t="s">
-        <v>72</v>
-      </c>
-      <c r="E91" t="s">
-        <v>385</v>
       </c>
       <c r="F91">
         <v>80</v>
       </c>
       <c r="G91" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H91" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I91">
         <v>92.543854494225997</v>
@@ -4702,25 +4724,25 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
+        <v>386</v>
+      </c>
+      <c r="C92" t="s">
         <v>387</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D92" t="s">
         <v>388</v>
       </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
         <v>389</v>
-      </c>
-      <c r="E92" t="s">
-        <v>390</v>
       </c>
       <c r="F92">
         <v>83</v>
       </c>
       <c r="G92" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H92" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I92">
         <v>93.320372344576001</v>
@@ -4735,25 +4757,25 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
+        <v>391</v>
+      </c>
+      <c r="C93" t="s">
         <v>392</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D93" t="s">
         <v>393</v>
       </c>
-      <c r="D93" t="s">
+      <c r="E93" t="s">
         <v>394</v>
-      </c>
-      <c r="E93" t="s">
-        <v>395</v>
       </c>
       <c r="F93">
         <v>79</v>
       </c>
       <c r="G93" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H93" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I93">
         <v>84.065129127237995</v>
@@ -4768,25 +4790,25 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
+        <v>396</v>
+      </c>
+      <c r="C94" t="s">
         <v>397</v>
       </c>
-      <c r="C94" t="s">
+      <c r="D94" t="s">
         <v>398</v>
       </c>
-      <c r="D94" t="s">
+      <c r="E94" t="s">
         <v>399</v>
-      </c>
-      <c r="E94" t="s">
-        <v>400</v>
       </c>
       <c r="F94">
         <v>87</v>
       </c>
       <c r="G94" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H94" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I94">
         <v>71.441191820802004</v>
@@ -4801,25 +4823,25 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
+        <v>401</v>
+      </c>
+      <c r="C95" t="s">
         <v>402</v>
       </c>
-      <c r="C95" t="s">
+      <c r="D95" t="s">
         <v>403</v>
       </c>
-      <c r="D95" t="s">
+      <c r="E95" t="s">
         <v>404</v>
-      </c>
-      <c r="E95" t="s">
-        <v>405</v>
       </c>
       <c r="F95">
         <v>78</v>
       </c>
       <c r="G95" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H95" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I95">
         <v>91.745275031375996</v>
@@ -4834,25 +4856,25 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
+        <v>406</v>
+      </c>
+      <c r="C96" t="s">
         <v>407</v>
       </c>
-      <c r="C96" t="s">
+      <c r="D96" t="s">
         <v>408</v>
       </c>
-      <c r="D96" t="s">
+      <c r="E96" t="s">
         <v>409</v>
-      </c>
-      <c r="E96" t="s">
-        <v>410</v>
       </c>
       <c r="F96">
         <v>82</v>
       </c>
       <c r="G96" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H96" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I96">
         <v>89.664344668335005</v>
@@ -4867,25 +4889,25 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
+        <v>411</v>
+      </c>
+      <c r="C97" t="s">
         <v>412</v>
       </c>
-      <c r="C97" t="s">
+      <c r="D97" t="s">
         <v>413</v>
       </c>
-      <c r="D97" t="s">
+      <c r="E97" t="s">
         <v>414</v>
-      </c>
-      <c r="E97" t="s">
-        <v>415</v>
       </c>
       <c r="F97">
         <v>85</v>
       </c>
       <c r="G97" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H97" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I97">
         <v>97.600723107636</v>
@@ -4900,25 +4922,25 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
+        <v>416</v>
+      </c>
+      <c r="C98" t="s">
         <v>417</v>
       </c>
-      <c r="C98" t="s">
+      <c r="D98" t="s">
         <v>418</v>
       </c>
-      <c r="D98" t="s">
+      <c r="E98" t="s">
         <v>419</v>
-      </c>
-      <c r="E98" t="s">
-        <v>420</v>
       </c>
       <c r="F98">
         <v>75</v>
       </c>
       <c r="G98" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H98" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I98">
         <v>86.645145380279999</v>
@@ -4933,25 +4955,25 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
+        <v>421</v>
+      </c>
+      <c r="C99" t="s">
         <v>422</v>
       </c>
-      <c r="C99" t="s">
+      <c r="D99" t="s">
         <v>423</v>
       </c>
-      <c r="D99" t="s">
+      <c r="E99" t="s">
         <v>424</v>
-      </c>
-      <c r="E99" t="s">
-        <v>425</v>
       </c>
       <c r="F99">
         <v>72</v>
       </c>
       <c r="G99" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H99" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I99">
         <v>92.886821627497994</v>
@@ -4966,25 +4988,25 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
+        <v>426</v>
+      </c>
+      <c r="C100" t="s">
         <v>427</v>
       </c>
-      <c r="C100" t="s">
+      <c r="D100" t="s">
         <v>428</v>
       </c>
-      <c r="D100" t="s">
+      <c r="E100" t="s">
         <v>429</v>
-      </c>
-      <c r="E100" t="s">
-        <v>430</v>
       </c>
       <c r="F100">
         <v>80</v>
       </c>
       <c r="G100" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H100" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I100">
         <v>82.793097985244998</v>
@@ -4999,25 +5021,25 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
+        <v>431</v>
+      </c>
+      <c r="C101" t="s">
         <v>432</v>
       </c>
-      <c r="C101" t="s">
+      <c r="D101" t="s">
         <v>433</v>
       </c>
-      <c r="D101" t="s">
+      <c r="E101" t="s">
         <v>434</v>
-      </c>
-      <c r="E101" t="s">
-        <v>435</v>
       </c>
       <c r="F101">
         <v>70</v>
       </c>
       <c r="G101" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H101" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I101">
         <v>87.155796755574997</v>

</xml_diff>